<commit_message>
last details from the diplexer codes
</commit_message>
<xml_diff>
--- a/masks/code/diplexer_FINAL_reformating.xlsx
+++ b/masks/code/diplexer_FINAL_reformating.xlsx
@@ -4515,13 +4515,11 @@
         <v>24.31</v>
       </c>
       <c r="Y60" s="1" t="n">
-        <v>-0</v>
+        <v>24.31</v>
       </c>
       <c r="Z60" s="1" t="n"/>
       <c r="AA60" s="1" t="n"/>
-      <c r="AB60" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="AB60" s="1" t="s"/>
     </row>
     <row r="61" spans="1:28">
       <c r="A61" s="1" t="s">
@@ -4589,13 +4587,11 @@
         <v>24.31</v>
       </c>
       <c r="Y61" s="1" t="n">
-        <v>-0</v>
+        <v>24.31</v>
       </c>
       <c r="Z61" s="1" t="n"/>
       <c r="AA61" s="1" t="n"/>
-      <c r="AB61" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="AB61" s="1" t="s"/>
     </row>
     <row r="62" spans="1:28">
       <c r="A62" s="1" t="s">
@@ -7646,10 +7642,10 @@
         <v>-42</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>-36.213</v>
+        <v>-47.787</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>5.787</v>
+        <v>-5.787</v>
       </c>
       <c r="N3" s="1" t="n"/>
       <c r="O3" s="1" t="n">
@@ -7659,10 +7655,10 @@
         <v>42</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>35.735</v>
+        <v>48.265</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-6.265</v>
+        <v>6.265</v>
       </c>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
@@ -7691,10 +7687,10 @@
         <v>-30</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>-34.857</v>
+        <v>-25.143</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>-4.857</v>
+        <v>4.857</v>
       </c>
       <c r="N4" s="1" t="n"/>
       <c r="O4" s="1" t="n">
@@ -7704,10 +7700,10 @@
         <v>30</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>35.335</v>
+        <v>24.665</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>5.335</v>
+        <v>-5.335</v>
       </c>
       <c r="S4" s="1" t="n"/>
       <c r="T4" s="1" t="n"/>
@@ -7736,10 +7732,10 @@
         <v>-18</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>-12.523</v>
+        <v>-23.477</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>5.477</v>
+        <v>-5.477</v>
       </c>
       <c r="N5" s="1" t="n"/>
       <c r="O5" s="1" t="n">
@@ -7749,10 +7745,10 @@
         <v>18</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>12.045</v>
+        <v>23.955</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-5.955</v>
+        <v>5.955</v>
       </c>
       <c r="S5" s="1" t="n"/>
       <c r="T5" s="1" t="n"/>
@@ -7781,10 +7777,10 @@
         <v>-6</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>-11.167</v>
+        <v>-0.833</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>-5.167</v>
+        <v>5.167</v>
       </c>
       <c r="N6" s="1" t="n"/>
       <c r="O6" s="1" t="n">
@@ -7794,10 +7790,10 @@
         <v>6</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>11.645</v>
+        <v>0.355</v>
       </c>
       <c r="R6" s="1" t="n">
-        <v>5.645</v>
+        <v>-5.645</v>
       </c>
       <c r="S6" s="1" t="n"/>
       <c r="T6" s="1" t="n"/>
@@ -7826,10 +7822,10 @@
         <v>6</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>11.167</v>
+        <v>0.833</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>5.167</v>
+        <v>-5.167</v>
       </c>
       <c r="N7" s="1" t="n"/>
       <c r="O7" s="1" t="n">
@@ -7839,10 +7835,10 @@
         <v>-6</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>-11.645</v>
+        <v>-0.355</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-5.645</v>
+        <v>5.645</v>
       </c>
       <c r="S7" s="1" t="n"/>
       <c r="T7" s="1" t="n"/>
@@ -7871,10 +7867,10 @@
         <v>18</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>12.523</v>
+        <v>23.477</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>-5.477</v>
+        <v>5.477</v>
       </c>
       <c r="N8" s="1" t="n"/>
       <c r="O8" s="1" t="n">
@@ -7884,10 +7880,10 @@
         <v>-18</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>-12.045</v>
+        <v>-23.955</v>
       </c>
       <c r="R8" s="1" t="n">
-        <v>5.955</v>
+        <v>-5.955</v>
       </c>
       <c r="S8" s="1" t="n"/>
       <c r="T8" s="1" t="n"/>
@@ -7916,10 +7912,10 @@
         <v>30</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>34.857</v>
+        <v>25.143</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>4.857</v>
+        <v>-4.857</v>
       </c>
       <c r="N9" s="1" t="n"/>
       <c r="O9" s="1" t="n">
@@ -7929,10 +7925,10 @@
         <v>-30</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>-35.335</v>
+        <v>-24.665</v>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-5.335</v>
+        <v>5.335</v>
       </c>
       <c r="S9" s="1" t="n"/>
       <c r="T9" s="1" t="n"/>
@@ -7961,10 +7957,10 @@
         <v>42</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>36.213</v>
+        <v>47.787</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>-5.787</v>
+        <v>5.787</v>
       </c>
       <c r="N10" s="1" t="n"/>
       <c r="O10" s="1" t="n">
@@ -7974,10 +7970,10 @@
         <v>-42</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>-35.735</v>
+        <v>-48.265</v>
       </c>
       <c r="R10" s="1" t="n">
-        <v>6.265</v>
+        <v>-6.265</v>
       </c>
       <c r="S10" s="1" t="n"/>
       <c r="T10" s="1" t="n"/>
@@ -8080,10 +8076,10 @@
         <v>-42</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>-41.955</v>
+        <v>-42.045</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.045</v>
+        <v>-0.045</v>
       </c>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n">
@@ -8093,10 +8089,10 @@
         <v>42</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>41.955</v>
+        <v>42.045</v>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.045</v>
+        <v>0.045</v>
       </c>
       <c r="S13" s="1" t="n"/>
       <c r="T13" s="1" t="n"/>
@@ -8125,10 +8121,10 @@
         <v>-30</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>-29.115</v>
+        <v>-30.885</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.885</v>
+        <v>-0.885</v>
       </c>
       <c r="N14" s="1" t="n"/>
       <c r="O14" s="1" t="n">
@@ -8138,10 +8134,10 @@
         <v>30</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>29.115</v>
+        <v>30.885</v>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.885</v>
+        <v>0.885</v>
       </c>
       <c r="S14" s="1" t="n"/>
       <c r="T14" s="1" t="n"/>
@@ -8170,10 +8166,10 @@
         <v>-18</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>-18.265</v>
+        <v>-17.735</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>-0.265</v>
+        <v>0.265</v>
       </c>
       <c r="N15" s="1" t="n"/>
       <c r="O15" s="1" t="n">
@@ -8183,10 +8179,10 @@
         <v>18</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>18.265</v>
+        <v>17.735</v>
       </c>
       <c r="R15" s="1" t="n">
-        <v>0.265</v>
+        <v>-0.265</v>
       </c>
       <c r="S15" s="1" t="n"/>
       <c r="T15" s="1" t="n"/>
@@ -8215,10 +8211,10 @@
         <v>-6</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>-5.425</v>
+        <v>-6.575</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>0.575</v>
+        <v>-0.575</v>
       </c>
       <c r="N16" s="1" t="n"/>
       <c r="O16" s="1" t="n">
@@ -8228,10 +8224,10 @@
         <v>6</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>5.425</v>
+        <v>6.575</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-0.575</v>
+        <v>0.575</v>
       </c>
       <c r="S16" s="1" t="n"/>
       <c r="T16" s="1" t="n"/>
@@ -8260,10 +8256,10 @@
         <v>6</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>5.425</v>
+        <v>6.575</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>-0.575</v>
+        <v>0.575</v>
       </c>
       <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n">
@@ -8273,10 +8269,10 @@
         <v>-6</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>-5.425</v>
+        <v>-6.575</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>0.575</v>
+        <v>-0.575</v>
       </c>
       <c r="S17" s="1" t="n"/>
       <c r="T17" s="1" t="n"/>
@@ -8305,10 +8301,10 @@
         <v>18</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>18.265</v>
+        <v>17.735</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.265</v>
+        <v>-0.265</v>
       </c>
       <c r="N18" s="1" t="n"/>
       <c r="O18" s="1" t="n">
@@ -8318,10 +8314,10 @@
         <v>-18</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>-18.265</v>
+        <v>-17.735</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.265</v>
+        <v>0.265</v>
       </c>
       <c r="S18" s="1" t="n"/>
       <c r="T18" s="1" t="n"/>
@@ -8350,10 +8346,10 @@
         <v>30</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>29.115</v>
+        <v>30.885</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>-0.885</v>
+        <v>0.885</v>
       </c>
       <c r="N19" s="1" t="n"/>
       <c r="O19" s="1" t="n">
@@ -8363,10 +8359,10 @@
         <v>-30</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>-29.115</v>
+        <v>-30.885</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0.885</v>
+        <v>-0.885</v>
       </c>
       <c r="S19" s="1" t="n"/>
       <c r="T19" s="1" t="n"/>
@@ -8395,10 +8391,10 @@
         <v>42</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>41.955</v>
+        <v>42.045</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>-0.045</v>
+        <v>0.045</v>
       </c>
       <c r="N20" s="1" t="n"/>
       <c r="O20" s="1" t="n">
@@ -8408,10 +8404,10 @@
         <v>-42</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>-41.955</v>
+        <v>-42.045</v>
       </c>
       <c r="R20" s="1" t="n">
-        <v>0.045</v>
+        <v>-0.045</v>
       </c>
       <c r="S20" s="1" t="n"/>
       <c r="T20" s="1" t="n"/>
@@ -8514,10 +8510,10 @@
         <v>-42</v>
       </c>
       <c r="L23" s="1" t="n">
-        <v>-36.213</v>
+        <v>-47.787</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>5.787</v>
+        <v>-5.787</v>
       </c>
       <c r="N23" s="1" t="n"/>
       <c r="O23" s="1" t="n">
@@ -8527,10 +8523,10 @@
         <v>42</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>35.735</v>
+        <v>48.265</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-6.265</v>
+        <v>6.265</v>
       </c>
       <c r="S23" s="1" t="n"/>
       <c r="T23" s="1" t="n"/>
@@ -8559,10 +8555,10 @@
         <v>-30</v>
       </c>
       <c r="L24" s="1" t="n">
-        <v>-34.857</v>
+        <v>-25.143</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>-4.857</v>
+        <v>4.857</v>
       </c>
       <c r="N24" s="1" t="n"/>
       <c r="O24" s="1" t="n">
@@ -8572,10 +8568,10 @@
         <v>30</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>35.335</v>
+        <v>24.665</v>
       </c>
       <c r="R24" s="1" t="n">
-        <v>5.335</v>
+        <v>-5.335</v>
       </c>
       <c r="S24" s="1" t="n"/>
       <c r="T24" s="1" t="n"/>
@@ -8604,10 +8600,10 @@
         <v>-18</v>
       </c>
       <c r="L25" s="1" t="n">
-        <v>-12.523</v>
+        <v>-23.477</v>
       </c>
       <c r="M25" s="1" t="n">
-        <v>5.477</v>
+        <v>-5.477</v>
       </c>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n">
@@ -8617,10 +8613,10 @@
         <v>18</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>12.045</v>
+        <v>23.955</v>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-5.955</v>
+        <v>5.955</v>
       </c>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
@@ -8649,10 +8645,10 @@
         <v>-6</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>-11.167</v>
+        <v>-0.833</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>-5.167</v>
+        <v>5.167</v>
       </c>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n">
@@ -8662,10 +8658,10 @@
         <v>6</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>11.645</v>
+        <v>0.355</v>
       </c>
       <c r="R26" s="1" t="n">
-        <v>5.645</v>
+        <v>-5.645</v>
       </c>
       <c r="S26" s="1" t="n"/>
       <c r="T26" s="1" t="n"/>
@@ -8694,10 +8690,10 @@
         <v>6</v>
       </c>
       <c r="L27" s="1" t="n">
-        <v>11.167</v>
+        <v>0.833</v>
       </c>
       <c r="M27" s="1" t="n">
-        <v>5.167</v>
+        <v>-5.167</v>
       </c>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n">
@@ -8707,10 +8703,10 @@
         <v>-6</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>-11.645</v>
+        <v>-0.355</v>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-5.645</v>
+        <v>5.645</v>
       </c>
       <c r="S27" s="1" t="n"/>
       <c r="T27" s="1" t="n"/>
@@ -8739,10 +8735,10 @@
         <v>18</v>
       </c>
       <c r="L28" s="1" t="n">
-        <v>12.523</v>
+        <v>23.477</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>-5.477</v>
+        <v>5.477</v>
       </c>
       <c r="N28" s="1" t="n"/>
       <c r="O28" s="1" t="n">
@@ -8752,10 +8748,10 @@
         <v>-18</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>-12.045</v>
+        <v>-23.955</v>
       </c>
       <c r="R28" s="1" t="n">
-        <v>5.955</v>
+        <v>-5.955</v>
       </c>
       <c r="S28" s="1" t="n"/>
       <c r="T28" s="1" t="n"/>
@@ -8784,10 +8780,10 @@
         <v>30</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>34.857</v>
+        <v>25.143</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>4.857</v>
+        <v>-4.857</v>
       </c>
       <c r="N29" s="1" t="n"/>
       <c r="O29" s="1" t="n">
@@ -8797,10 +8793,10 @@
         <v>-30</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>-35.335</v>
+        <v>-24.665</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-5.335</v>
+        <v>5.335</v>
       </c>
       <c r="S29" s="1" t="n"/>
       <c r="T29" s="1" t="n"/>
@@ -8829,10 +8825,10 @@
         <v>42</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>36.213</v>
+        <v>47.787</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>-5.787</v>
+        <v>5.787</v>
       </c>
       <c r="N30" s="1" t="n"/>
       <c r="O30" s="1" t="n">
@@ -8842,10 +8838,10 @@
         <v>-42</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>-35.735</v>
+        <v>-48.265</v>
       </c>
       <c r="R30" s="1" t="n">
-        <v>6.265</v>
+        <v>-6.265</v>
       </c>
       <c r="S30" s="1" t="n"/>
       <c r="T30" s="1" t="n"/>
@@ -8917,7 +8913,7 @@
     </row>
     <row r="33" spans="1:27">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>59</v>
@@ -8926,7 +8922,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>0</v>
@@ -8938,7 +8934,7 @@
         <v>24.31</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>-0</v>
+        <v>12</v>
       </c>
       <c r="I33" s="1" t="n"/>
       <c r="J33" s="1" t="n">
@@ -8958,13 +8954,13 @@
         <v>1</v>
       </c>
       <c r="P33" s="1" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>-36.465</v>
+        <v>48.265</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>-36.465</v>
+        <v>6.265</v>
       </c>
       <c r="S33" s="1" t="n"/>
       <c r="T33" s="1" t="n"/>
@@ -9003,13 +8999,13 @@
         <v>2</v>
       </c>
       <c r="P34" s="1" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>-12.155</v>
+        <v>24.665</v>
       </c>
       <c r="R34" s="1" t="n">
-        <v>-12.155</v>
+        <v>-5.335</v>
       </c>
       <c r="S34" s="1" t="n"/>
       <c r="T34" s="1" t="n"/>
@@ -9048,13 +9044,13 @@
         <v>3</v>
       </c>
       <c r="P35" s="1" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="Q35" s="1" t="n">
-        <v>12.155</v>
+        <v>23.955</v>
       </c>
       <c r="R35" s="1" t="n">
-        <v>12.155</v>
+        <v>5.955</v>
       </c>
       <c r="S35" s="1" t="n"/>
       <c r="T35" s="1" t="n"/>
@@ -9093,13 +9089,13 @@
         <v>4</v>
       </c>
       <c r="P36" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>36.465</v>
+        <v>0.355</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>36.465</v>
+        <v>-5.645</v>
       </c>
       <c r="S36" s="1" t="n"/>
       <c r="T36" s="1" t="n"/>
@@ -9126,10 +9122,18 @@
       <c r="L37" s="1" t="n"/>
       <c r="M37" s="1" t="n"/>
       <c r="N37" s="1" t="n"/>
-      <c r="O37" s="1" t="n"/>
-      <c r="P37" s="1" t="n"/>
-      <c r="Q37" s="1" t="n"/>
-      <c r="R37" s="1" t="n"/>
+      <c r="O37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P37" s="1" t="n">
+        <v>-6</v>
+      </c>
+      <c r="Q37" s="1" t="n">
+        <v>-0.355</v>
+      </c>
+      <c r="R37" s="1" t="n">
+        <v>5.645</v>
+      </c>
       <c r="S37" s="1" t="n"/>
       <c r="T37" s="1" t="n"/>
       <c r="U37" s="1" t="n"/>
@@ -9155,10 +9159,18 @@
       <c r="L38" s="1" t="n"/>
       <c r="M38" s="1" t="n"/>
       <c r="N38" s="1" t="n"/>
-      <c r="O38" s="1" t="n"/>
-      <c r="P38" s="1" t="n"/>
-      <c r="Q38" s="1" t="n"/>
-      <c r="R38" s="1" t="n"/>
+      <c r="O38" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>-18</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>-23.955</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <v>-5.955</v>
+      </c>
       <c r="S38" s="1" t="n"/>
       <c r="T38" s="1" t="n"/>
       <c r="U38" s="1" t="n"/>
@@ -9170,55 +9182,31 @@
       <c r="AA38" s="1" t="n"/>
     </row>
     <row r="39" spans="1:27">
-      <c r="A39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>-0</v>
-      </c>
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="n"/>
+      <c r="D39" s="1" t="n"/>
+      <c r="E39" s="1" t="n"/>
+      <c r="F39" s="1" t="n"/>
+      <c r="G39" s="1" t="n"/>
+      <c r="H39" s="1" t="n"/>
       <c r="I39" s="1" t="n"/>
-      <c r="J39" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J39" s="1" t="n"/>
+      <c r="K39" s="1" t="n"/>
+      <c r="L39" s="1" t="n"/>
+      <c r="M39" s="1" t="n"/>
       <c r="N39" s="1" t="n"/>
       <c r="O39" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P39" s="1" t="n">
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="Q39" s="1" t="n">
-        <v>-36.465</v>
+        <v>-24.665</v>
       </c>
       <c r="R39" s="1" t="n">
-        <v>-36.465</v>
+        <v>5.335</v>
       </c>
       <c r="S39" s="1" t="n"/>
       <c r="T39" s="1" t="n"/>
@@ -9240,30 +9228,22 @@
       <c r="G40" s="1" t="n"/>
       <c r="H40" s="1" t="n"/>
       <c r="I40" s="1" t="n"/>
-      <c r="J40" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K40" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J40" s="1" t="n"/>
+      <c r="K40" s="1" t="n"/>
+      <c r="L40" s="1" t="n"/>
+      <c r="M40" s="1" t="n"/>
       <c r="N40" s="1" t="n"/>
       <c r="O40" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P40" s="1" t="n">
-        <v>0</v>
+        <v>-42</v>
       </c>
       <c r="Q40" s="1" t="n">
-        <v>-12.155</v>
+        <v>-48.265</v>
       </c>
       <c r="R40" s="1" t="n">
-        <v>-12.155</v>
+        <v>-6.265</v>
       </c>
       <c r="S40" s="1" t="n"/>
       <c r="T40" s="1" t="n"/>
@@ -9285,31 +9265,15 @@
       <c r="G41" s="1" t="n"/>
       <c r="H41" s="1" t="n"/>
       <c r="I41" s="1" t="n"/>
-      <c r="J41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J41" s="1" t="n"/>
+      <c r="K41" s="1" t="n"/>
+      <c r="L41" s="1" t="n"/>
+      <c r="M41" s="1" t="n"/>
       <c r="N41" s="1" t="n"/>
-      <c r="O41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="1" t="n">
-        <v>12.155</v>
-      </c>
-      <c r="R41" s="1" t="n">
-        <v>12.155</v>
-      </c>
+      <c r="O41" s="1" t="n"/>
+      <c r="P41" s="1" t="n"/>
+      <c r="Q41" s="1" t="n"/>
+      <c r="R41" s="1" t="n"/>
       <c r="S41" s="1" t="n"/>
       <c r="T41" s="1" t="n"/>
       <c r="U41" s="1" t="n"/>
@@ -9330,31 +9294,15 @@
       <c r="G42" s="1" t="n"/>
       <c r="H42" s="1" t="n"/>
       <c r="I42" s="1" t="n"/>
-      <c r="J42" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J42" s="1" t="n"/>
+      <c r="K42" s="1" t="n"/>
+      <c r="L42" s="1" t="n"/>
+      <c r="M42" s="1" t="n"/>
       <c r="N42" s="1" t="n"/>
-      <c r="O42" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="1" t="n">
-        <v>36.465</v>
-      </c>
-      <c r="R42" s="1" t="n">
-        <v>36.465</v>
-      </c>
+      <c r="O42" s="1" t="n"/>
+      <c r="P42" s="1" t="n"/>
+      <c r="Q42" s="1" t="n"/>
+      <c r="R42" s="1" t="n"/>
       <c r="S42" s="1" t="n"/>
       <c r="T42" s="1" t="n"/>
       <c r="U42" s="1" t="n"/>
@@ -9366,24 +9314,56 @@
       <c r="AA42" s="1" t="n"/>
     </row>
     <row r="43" spans="1:27">
-      <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="n"/>
-      <c r="D43" s="1" t="n"/>
-      <c r="E43" s="1" t="n"/>
-      <c r="F43" s="1" t="n"/>
-      <c r="G43" s="1" t="n"/>
-      <c r="H43" s="1" t="n"/>
+      <c r="A43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>24.31</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="I43" s="1" t="n"/>
-      <c r="J43" s="1" t="n"/>
-      <c r="K43" s="1" t="n"/>
-      <c r="L43" s="1" t="n"/>
-      <c r="M43" s="1" t="n"/>
+      <c r="J43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N43" s="1" t="n"/>
-      <c r="O43" s="1" t="n"/>
-      <c r="P43" s="1" t="n"/>
-      <c r="Q43" s="1" t="n"/>
-      <c r="R43" s="1" t="n"/>
+      <c r="O43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P43" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="1" t="n">
+        <v>43.905</v>
+      </c>
+      <c r="R43" s="1" t="n">
+        <v>-0.095</v>
+      </c>
       <c r="S43" s="1" t="n"/>
       <c r="T43" s="1" t="n"/>
       <c r="U43" s="1" t="n"/>
@@ -9404,15 +9384,31 @@
       <c r="G44" s="1" t="n"/>
       <c r="H44" s="1" t="n"/>
       <c r="I44" s="1" t="n"/>
-      <c r="J44" s="1" t="n"/>
-      <c r="K44" s="1" t="n"/>
-      <c r="L44" s="1" t="n"/>
-      <c r="M44" s="1" t="n"/>
+      <c r="J44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N44" s="1" t="n"/>
-      <c r="O44" s="1" t="n"/>
-      <c r="P44" s="1" t="n"/>
-      <c r="Q44" s="1" t="n"/>
-      <c r="R44" s="1" t="n"/>
+      <c r="O44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="P44" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q44" s="1" t="n">
+        <v>36.465</v>
+      </c>
+      <c r="R44" s="1" t="n">
+        <v>0.465</v>
+      </c>
       <c r="S44" s="1" t="n"/>
       <c r="T44" s="1" t="n"/>
       <c r="U44" s="1" t="n"/>
@@ -9424,33 +9420,17 @@
       <c r="AA44" s="1" t="n"/>
     </row>
     <row r="45" spans="1:27">
-      <c r="A45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E45" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="H45" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="A45" s="1" t="n"/>
+      <c r="B45" s="1" t="n"/>
+      <c r="C45" s="1" t="n"/>
+      <c r="D45" s="1" t="n"/>
+      <c r="E45" s="1" t="n"/>
+      <c r="F45" s="1" t="n"/>
+      <c r="G45" s="1" t="n"/>
+      <c r="H45" s="1" t="n"/>
       <c r="I45" s="1" t="n"/>
       <c r="J45" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K45" s="1" t="n">
         <v>0</v>
@@ -9463,16 +9443,16 @@
       </c>
       <c r="N45" s="1" t="n"/>
       <c r="O45" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P45" s="1" t="n">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="Q45" s="1" t="n">
-        <v>35.735</v>
+        <v>29.025</v>
       </c>
       <c r="R45" s="1" t="n">
-        <v>-6.265</v>
+        <v>1.025</v>
       </c>
       <c r="S45" s="1" t="n"/>
       <c r="T45" s="1" t="n"/>
@@ -9495,7 +9475,7 @@
       <c r="H46" s="1" t="n"/>
       <c r="I46" s="1" t="n"/>
       <c r="J46" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K46" s="1" t="n">
         <v>0</v>
@@ -9508,16 +9488,16 @@
       </c>
       <c r="N46" s="1" t="n"/>
       <c r="O46" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P46" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q46" s="1" t="n">
-        <v>35.335</v>
+        <v>19.595</v>
       </c>
       <c r="R46" s="1" t="n">
-        <v>5.335</v>
+        <v>-0.405</v>
       </c>
       <c r="S46" s="1" t="n"/>
       <c r="T46" s="1" t="n"/>
@@ -9539,30 +9519,22 @@
       <c r="G47" s="1" t="n"/>
       <c r="H47" s="1" t="n"/>
       <c r="I47" s="1" t="n"/>
-      <c r="J47" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J47" s="1" t="n"/>
+      <c r="K47" s="1" t="n"/>
+      <c r="L47" s="1" t="n"/>
+      <c r="M47" s="1" t="n"/>
       <c r="N47" s="1" t="n"/>
       <c r="O47" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P47" s="1" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q47" s="1" t="n">
-        <v>12.045</v>
+        <v>12.155</v>
       </c>
       <c r="R47" s="1" t="n">
-        <v>-5.955</v>
+        <v>0.155</v>
       </c>
       <c r="S47" s="1" t="n"/>
       <c r="T47" s="1" t="n"/>
@@ -9584,30 +9556,22 @@
       <c r="G48" s="1" t="n"/>
       <c r="H48" s="1" t="n"/>
       <c r="I48" s="1" t="n"/>
-      <c r="J48" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K48" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J48" s="1" t="n"/>
+      <c r="K48" s="1" t="n"/>
+      <c r="L48" s="1" t="n"/>
+      <c r="M48" s="1" t="n"/>
       <c r="N48" s="1" t="n"/>
       <c r="O48" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="P48" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="P48" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="Q48" s="1" t="n">
-        <v>11.645</v>
+        <v>4.715</v>
       </c>
       <c r="R48" s="1" t="n">
-        <v>5.645</v>
+        <v>0.715</v>
       </c>
       <c r="S48" s="1" t="n"/>
       <c r="T48" s="1" t="n"/>
@@ -9635,16 +9599,16 @@
       <c r="M49" s="1" t="n"/>
       <c r="N49" s="1" t="n"/>
       <c r="O49" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P49" s="1" t="n">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="Q49" s="1" t="n">
-        <v>-11.645</v>
+        <v>-4.715</v>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-5.645</v>
+        <v>-0.715</v>
       </c>
       <c r="S49" s="1" t="n"/>
       <c r="T49" s="1" t="n"/>
@@ -9672,16 +9636,16 @@
       <c r="M50" s="1" t="n"/>
       <c r="N50" s="1" t="n"/>
       <c r="O50" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P50" s="1" t="n">
-        <v>-18</v>
+        <v>-12</v>
       </c>
       <c r="Q50" s="1" t="n">
-        <v>-12.045</v>
+        <v>-12.155</v>
       </c>
       <c r="R50" s="1" t="n">
-        <v>5.955</v>
+        <v>-0.155</v>
       </c>
       <c r="S50" s="1" t="n"/>
       <c r="T50" s="1" t="n"/>
@@ -9709,16 +9673,16 @@
       <c r="M51" s="1" t="n"/>
       <c r="N51" s="1" t="n"/>
       <c r="O51" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P51" s="1" t="n">
-        <v>-30</v>
+        <v>-20</v>
       </c>
       <c r="Q51" s="1" t="n">
-        <v>-35.335</v>
+        <v>-19.595</v>
       </c>
       <c r="R51" s="1" t="n">
-        <v>-5.335</v>
+        <v>0.405</v>
       </c>
       <c r="S51" s="1" t="n"/>
       <c r="T51" s="1" t="n"/>
@@ -9746,16 +9710,16 @@
       <c r="M52" s="1" t="n"/>
       <c r="N52" s="1" t="n"/>
       <c r="O52" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P52" s="1" t="n">
-        <v>-42</v>
+        <v>-28</v>
       </c>
       <c r="Q52" s="1" t="n">
-        <v>-35.735</v>
+        <v>-29.025</v>
       </c>
       <c r="R52" s="1" t="n">
-        <v>6.265</v>
+        <v>-1.025</v>
       </c>
       <c r="S52" s="1" t="n"/>
       <c r="T52" s="1" t="n"/>
@@ -9782,10 +9746,18 @@
       <c r="L53" s="1" t="n"/>
       <c r="M53" s="1" t="n"/>
       <c r="N53" s="1" t="n"/>
-      <c r="O53" s="1" t="n"/>
-      <c r="P53" s="1" t="n"/>
-      <c r="Q53" s="1" t="n"/>
-      <c r="R53" s="1" t="n"/>
+      <c r="O53" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="P53" s="1" t="n">
+        <v>-36</v>
+      </c>
+      <c r="Q53" s="1" t="n">
+        <v>-36.465</v>
+      </c>
+      <c r="R53" s="1" t="n">
+        <v>-0.465</v>
+      </c>
       <c r="S53" s="1" t="n"/>
       <c r="T53" s="1" t="n"/>
       <c r="U53" s="1" t="n"/>
@@ -9811,10 +9783,18 @@
       <c r="L54" s="1" t="n"/>
       <c r="M54" s="1" t="n"/>
       <c r="N54" s="1" t="n"/>
-      <c r="O54" s="1" t="n"/>
-      <c r="P54" s="1" t="n"/>
-      <c r="Q54" s="1" t="n"/>
-      <c r="R54" s="1" t="n"/>
+      <c r="O54" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P54" s="1" t="n">
+        <v>-44</v>
+      </c>
+      <c r="Q54" s="1" t="n">
+        <v>-43.905</v>
+      </c>
+      <c r="R54" s="1" t="n">
+        <v>0.095</v>
+      </c>
       <c r="S54" s="1" t="n"/>
       <c r="T54" s="1" t="n"/>
       <c r="U54" s="1" t="n"/>
@@ -9826,56 +9806,24 @@
       <c r="AA54" s="1" t="n"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="H55" s="1" t="n">
-        <v>8</v>
-      </c>
+      <c r="A55" s="1" t="n"/>
+      <c r="B55" s="1" t="n"/>
+      <c r="C55" s="1" t="n"/>
+      <c r="D55" s="1" t="n"/>
+      <c r="E55" s="1" t="n"/>
+      <c r="F55" s="1" t="n"/>
+      <c r="G55" s="1" t="n"/>
+      <c r="H55" s="1" t="n"/>
       <c r="I55" s="1" t="n"/>
-      <c r="J55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J55" s="1" t="n"/>
+      <c r="K55" s="1" t="n"/>
+      <c r="L55" s="1" t="n"/>
+      <c r="M55" s="1" t="n"/>
       <c r="N55" s="1" t="n"/>
-      <c r="O55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P55" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="Q55" s="1" t="n">
-        <v>44.095</v>
-      </c>
-      <c r="R55" s="1" t="n">
-        <v>0.095</v>
-      </c>
+      <c r="O55" s="1" t="n"/>
+      <c r="P55" s="1" t="n"/>
+      <c r="Q55" s="1" t="n"/>
+      <c r="R55" s="1" t="n"/>
       <c r="S55" s="1" t="n"/>
       <c r="T55" s="1" t="n"/>
       <c r="U55" s="1" t="n"/>
@@ -9896,31 +9844,15 @@
       <c r="G56" s="1" t="n"/>
       <c r="H56" s="1" t="n"/>
       <c r="I56" s="1" t="n"/>
-      <c r="J56" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J56" s="1" t="n"/>
+      <c r="K56" s="1" t="n"/>
+      <c r="L56" s="1" t="n"/>
+      <c r="M56" s="1" t="n"/>
       <c r="N56" s="1" t="n"/>
-      <c r="O56" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P56" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q56" s="1" t="n">
-        <v>35.535</v>
-      </c>
-      <c r="R56" s="1" t="n">
-        <v>-0.465</v>
-      </c>
+      <c r="O56" s="1" t="n"/>
+      <c r="P56" s="1" t="n"/>
+      <c r="Q56" s="1" t="n"/>
+      <c r="R56" s="1" t="n"/>
       <c r="S56" s="1" t="n"/>
       <c r="T56" s="1" t="n"/>
       <c r="U56" s="1" t="n"/>
@@ -9932,17 +9864,33 @@
       <c r="AA56" s="1" t="n"/>
     </row>
     <row r="57" spans="1:27">
-      <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="n"/>
-      <c r="D57" s="1" t="n"/>
-      <c r="E57" s="1" t="n"/>
-      <c r="F57" s="1" t="n"/>
-      <c r="G57" s="1" t="n"/>
-      <c r="H57" s="1" t="n"/>
+      <c r="A57" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>24.31</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="I57" s="1" t="n"/>
       <c r="J57" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K57" s="1" t="n">
         <v>0</v>
@@ -9955,16 +9903,16 @@
       </c>
       <c r="N57" s="1" t="n"/>
       <c r="O57" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P57" s="1" t="n">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="Q57" s="1" t="n">
-        <v>26.975</v>
+        <v>43.905</v>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-1.025</v>
+        <v>-0.095</v>
       </c>
       <c r="S57" s="1" t="n"/>
       <c r="T57" s="1" t="n"/>
@@ -9987,7 +9935,7 @@
       <c r="H58" s="1" t="n"/>
       <c r="I58" s="1" t="n"/>
       <c r="J58" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K58" s="1" t="n">
         <v>0</v>
@@ -10000,16 +9948,16 @@
       </c>
       <c r="N58" s="1" t="n"/>
       <c r="O58" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P58" s="1" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="Q58" s="1" t="n">
-        <v>20.405</v>
+        <v>36.465</v>
       </c>
       <c r="R58" s="1" t="n">
-        <v>0.405</v>
+        <v>0.465</v>
       </c>
       <c r="S58" s="1" t="n"/>
       <c r="T58" s="1" t="n"/>
@@ -10031,22 +9979,30 @@
       <c r="G59" s="1" t="n"/>
       <c r="H59" s="1" t="n"/>
       <c r="I59" s="1" t="n"/>
-      <c r="J59" s="1" t="n"/>
-      <c r="K59" s="1" t="n"/>
-      <c r="L59" s="1" t="n"/>
-      <c r="M59" s="1" t="n"/>
+      <c r="J59" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N59" s="1" t="n"/>
       <c r="O59" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>11.845</v>
+        <v>29.025</v>
       </c>
       <c r="R59" s="1" t="n">
-        <v>-0.155</v>
+        <v>1.025</v>
       </c>
       <c r="S59" s="1" t="n"/>
       <c r="T59" s="1" t="n"/>
@@ -10068,22 +10024,30 @@
       <c r="G60" s="1" t="n"/>
       <c r="H60" s="1" t="n"/>
       <c r="I60" s="1" t="n"/>
-      <c r="J60" s="1" t="n"/>
-      <c r="K60" s="1" t="n"/>
-      <c r="L60" s="1" t="n"/>
-      <c r="M60" s="1" t="n"/>
+      <c r="J60" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N60" s="1" t="n"/>
       <c r="O60" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P60" s="1" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="Q60" s="1" t="n">
-        <v>3.285</v>
+        <v>19.595</v>
       </c>
       <c r="R60" s="1" t="n">
-        <v>-0.715</v>
+        <v>-0.405</v>
       </c>
       <c r="S60" s="1" t="n"/>
       <c r="T60" s="1" t="n"/>
@@ -10111,16 +10075,16 @@
       <c r="M61" s="1" t="n"/>
       <c r="N61" s="1" t="n"/>
       <c r="O61" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>-4</v>
+        <v>12</v>
       </c>
       <c r="Q61" s="1" t="n">
-        <v>-3.285</v>
+        <v>12.155</v>
       </c>
       <c r="R61" s="1" t="n">
-        <v>0.715</v>
+        <v>0.155</v>
       </c>
       <c r="S61" s="1" t="n"/>
       <c r="T61" s="1" t="n"/>
@@ -10148,16 +10112,16 @@
       <c r="M62" s="1" t="n"/>
       <c r="N62" s="1" t="n"/>
       <c r="O62" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P62" s="1" t="n">
-        <v>-12</v>
+        <v>4</v>
       </c>
       <c r="Q62" s="1" t="n">
-        <v>-11.845</v>
+        <v>4.715</v>
       </c>
       <c r="R62" s="1" t="n">
-        <v>0.155</v>
+        <v>0.715</v>
       </c>
       <c r="S62" s="1" t="n"/>
       <c r="T62" s="1" t="n"/>
@@ -10185,16 +10149,16 @@
       <c r="M63" s="1" t="n"/>
       <c r="N63" s="1" t="n"/>
       <c r="O63" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P63" s="1" t="n">
-        <v>-20</v>
+        <v>-4</v>
       </c>
       <c r="Q63" s="1" t="n">
-        <v>-20.405</v>
+        <v>-4.715</v>
       </c>
       <c r="R63" s="1" t="n">
-        <v>-0.405</v>
+        <v>-0.715</v>
       </c>
       <c r="S63" s="1" t="n"/>
       <c r="T63" s="1" t="n"/>
@@ -10222,16 +10186,16 @@
       <c r="M64" s="1" t="n"/>
       <c r="N64" s="1" t="n"/>
       <c r="O64" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P64" s="1" t="n">
-        <v>-28</v>
+        <v>-12</v>
       </c>
       <c r="Q64" s="1" t="n">
-        <v>-26.975</v>
+        <v>-12.155</v>
       </c>
       <c r="R64" s="1" t="n">
-        <v>1.025</v>
+        <v>-0.155</v>
       </c>
       <c r="S64" s="1" t="n"/>
       <c r="T64" s="1" t="n"/>
@@ -10259,16 +10223,16 @@
       <c r="M65" s="1" t="n"/>
       <c r="N65" s="1" t="n"/>
       <c r="O65" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P65" s="1" t="n">
-        <v>-36</v>
+        <v>-20</v>
       </c>
       <c r="Q65" s="1" t="n">
-        <v>-35.535</v>
+        <v>-19.595</v>
       </c>
       <c r="R65" s="1" t="n">
-        <v>0.465</v>
+        <v>0.405</v>
       </c>
       <c r="S65" s="1" t="n"/>
       <c r="T65" s="1" t="n"/>
@@ -10296,16 +10260,16 @@
       <c r="M66" s="1" t="n"/>
       <c r="N66" s="1" t="n"/>
       <c r="O66" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P66" s="1" t="n">
-        <v>-44</v>
+        <v>-28</v>
       </c>
       <c r="Q66" s="1" t="n">
-        <v>-44.095</v>
+        <v>-29.025</v>
       </c>
       <c r="R66" s="1" t="n">
-        <v>-0.095</v>
+        <v>-1.025</v>
       </c>
       <c r="S66" s="1" t="n"/>
       <c r="T66" s="1" t="n"/>
@@ -10332,10 +10296,18 @@
       <c r="L67" s="1" t="n"/>
       <c r="M67" s="1" t="n"/>
       <c r="N67" s="1" t="n"/>
-      <c r="O67" s="1" t="n"/>
-      <c r="P67" s="1" t="n"/>
-      <c r="Q67" s="1" t="n"/>
-      <c r="R67" s="1" t="n"/>
+      <c r="O67" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="P67" s="1" t="n">
+        <v>-36</v>
+      </c>
+      <c r="Q67" s="1" t="n">
+        <v>-36.465</v>
+      </c>
+      <c r="R67" s="1" t="n">
+        <v>-0.465</v>
+      </c>
       <c r="S67" s="1" t="n"/>
       <c r="T67" s="1" t="n"/>
       <c r="U67" s="1" t="n"/>
@@ -10361,10 +10333,18 @@
       <c r="L68" s="1" t="n"/>
       <c r="M68" s="1" t="n"/>
       <c r="N68" s="1" t="n"/>
-      <c r="O68" s="1" t="n"/>
-      <c r="P68" s="1" t="n"/>
-      <c r="Q68" s="1" t="n"/>
-      <c r="R68" s="1" t="n"/>
+      <c r="O68" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P68" s="1" t="n">
+        <v>-44</v>
+      </c>
+      <c r="Q68" s="1" t="n">
+        <v>-43.905</v>
+      </c>
+      <c r="R68" s="1" t="n">
+        <v>0.095</v>
+      </c>
       <c r="S68" s="1" t="n"/>
       <c r="T68" s="1" t="n"/>
       <c r="U68" s="1" t="n"/>
@@ -10376,56 +10356,24 @@
       <c r="AA68" s="1" t="n"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D69" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="H69" s="1" t="n">
-        <v>8</v>
-      </c>
+      <c r="A69" s="1" t="n"/>
+      <c r="B69" s="1" t="n"/>
+      <c r="C69" s="1" t="n"/>
+      <c r="D69" s="1" t="n"/>
+      <c r="E69" s="1" t="n"/>
+      <c r="F69" s="1" t="n"/>
+      <c r="G69" s="1" t="n"/>
+      <c r="H69" s="1" t="n"/>
       <c r="I69" s="1" t="n"/>
-      <c r="J69" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M69" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J69" s="1" t="n"/>
+      <c r="K69" s="1" t="n"/>
+      <c r="L69" s="1" t="n"/>
+      <c r="M69" s="1" t="n"/>
       <c r="N69" s="1" t="n"/>
-      <c r="O69" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P69" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="Q69" s="1" t="n">
-        <v>44.095</v>
-      </c>
-      <c r="R69" s="1" t="n">
-        <v>0.095</v>
-      </c>
+      <c r="O69" s="1" t="n"/>
+      <c r="P69" s="1" t="n"/>
+      <c r="Q69" s="1" t="n"/>
+      <c r="R69" s="1" t="n"/>
       <c r="S69" s="1" t="n"/>
       <c r="T69" s="1" t="n"/>
       <c r="U69" s="1" t="n"/>
@@ -10446,31 +10394,15 @@
       <c r="G70" s="1" t="n"/>
       <c r="H70" s="1" t="n"/>
       <c r="I70" s="1" t="n"/>
-      <c r="J70" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K70" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L70" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M70" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J70" s="1" t="n"/>
+      <c r="K70" s="1" t="n"/>
+      <c r="L70" s="1" t="n"/>
+      <c r="M70" s="1" t="n"/>
       <c r="N70" s="1" t="n"/>
-      <c r="O70" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P70" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q70" s="1" t="n">
-        <v>35.535</v>
-      </c>
-      <c r="R70" s="1" t="n">
-        <v>-0.465</v>
-      </c>
+      <c r="O70" s="1" t="n"/>
+      <c r="P70" s="1" t="n"/>
+      <c r="Q70" s="1" t="n"/>
+      <c r="R70" s="1" t="n"/>
       <c r="S70" s="1" t="n"/>
       <c r="T70" s="1" t="n"/>
       <c r="U70" s="1" t="n"/>
@@ -10482,17 +10414,33 @@
       <c r="AA70" s="1" t="n"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n"/>
-      <c r="C71" s="1" t="n"/>
-      <c r="D71" s="1" t="n"/>
-      <c r="E71" s="1" t="n"/>
-      <c r="F71" s="1" t="n"/>
-      <c r="G71" s="1" t="n"/>
-      <c r="H71" s="1" t="n"/>
+      <c r="A71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="n">
+        <v>24.31</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <v>12</v>
+      </c>
       <c r="I71" s="1" t="n"/>
       <c r="J71" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K71" s="1" t="n">
         <v>0</v>
@@ -10505,16 +10453,16 @@
       </c>
       <c r="N71" s="1" t="n"/>
       <c r="O71" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P71" s="1" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="Q71" s="1" t="n">
-        <v>26.975</v>
+        <v>48.265</v>
       </c>
       <c r="R71" s="1" t="n">
-        <v>-1.025</v>
+        <v>6.265</v>
       </c>
       <c r="S71" s="1" t="n"/>
       <c r="T71" s="1" t="n"/>
@@ -10537,7 +10485,7 @@
       <c r="H72" s="1" t="n"/>
       <c r="I72" s="1" t="n"/>
       <c r="J72" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K72" s="1" t="n">
         <v>0</v>
@@ -10550,16 +10498,16 @@
       </c>
       <c r="N72" s="1" t="n"/>
       <c r="O72" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P72" s="1" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="Q72" s="1" t="n">
-        <v>20.405</v>
+        <v>24.665</v>
       </c>
       <c r="R72" s="1" t="n">
-        <v>0.405</v>
+        <v>-5.335</v>
       </c>
       <c r="S72" s="1" t="n"/>
       <c r="T72" s="1" t="n"/>
@@ -10581,22 +10529,30 @@
       <c r="G73" s="1" t="n"/>
       <c r="H73" s="1" t="n"/>
       <c r="I73" s="1" t="n"/>
-      <c r="J73" s="1" t="n"/>
-      <c r="K73" s="1" t="n"/>
-      <c r="L73" s="1" t="n"/>
-      <c r="M73" s="1" t="n"/>
+      <c r="J73" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N73" s="1" t="n"/>
       <c r="O73" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P73" s="1" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="Q73" s="1" t="n">
-        <v>11.845</v>
+        <v>23.955</v>
       </c>
       <c r="R73" s="1" t="n">
-        <v>-0.155</v>
+        <v>5.955</v>
       </c>
       <c r="S73" s="1" t="n"/>
       <c r="T73" s="1" t="n"/>
@@ -10618,22 +10574,30 @@
       <c r="G74" s="1" t="n"/>
       <c r="H74" s="1" t="n"/>
       <c r="I74" s="1" t="n"/>
-      <c r="J74" s="1" t="n"/>
-      <c r="K74" s="1" t="n"/>
-      <c r="L74" s="1" t="n"/>
-      <c r="M74" s="1" t="n"/>
+      <c r="J74" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N74" s="1" t="n"/>
       <c r="O74" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P74" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="P74" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="Q74" s="1" t="n">
-        <v>3.285</v>
+        <v>0.355</v>
       </c>
       <c r="R74" s="1" t="n">
-        <v>-0.715</v>
+        <v>-5.645</v>
       </c>
       <c r="S74" s="1" t="n"/>
       <c r="T74" s="1" t="n"/>
@@ -10661,16 +10625,16 @@
       <c r="M75" s="1" t="n"/>
       <c r="N75" s="1" t="n"/>
       <c r="O75" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P75" s="1" t="n">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="Q75" s="1" t="n">
-        <v>-3.285</v>
+        <v>-0.355</v>
       </c>
       <c r="R75" s="1" t="n">
-        <v>0.715</v>
+        <v>5.645</v>
       </c>
       <c r="S75" s="1" t="n"/>
       <c r="T75" s="1" t="n"/>
@@ -10698,16 +10662,16 @@
       <c r="M76" s="1" t="n"/>
       <c r="N76" s="1" t="n"/>
       <c r="O76" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P76" s="1" t="n">
-        <v>-12</v>
+        <v>-18</v>
       </c>
       <c r="Q76" s="1" t="n">
-        <v>-11.845</v>
+        <v>-23.955</v>
       </c>
       <c r="R76" s="1" t="n">
-        <v>0.155</v>
+        <v>-5.955</v>
       </c>
       <c r="S76" s="1" t="n"/>
       <c r="T76" s="1" t="n"/>
@@ -10735,16 +10699,16 @@
       <c r="M77" s="1" t="n"/>
       <c r="N77" s="1" t="n"/>
       <c r="O77" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P77" s="1" t="n">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="Q77" s="1" t="n">
-        <v>-20.405</v>
+        <v>-24.665</v>
       </c>
       <c r="R77" s="1" t="n">
-        <v>-0.405</v>
+        <v>5.335</v>
       </c>
       <c r="S77" s="1" t="n"/>
       <c r="T77" s="1" t="n"/>
@@ -10772,16 +10736,16 @@
       <c r="M78" s="1" t="n"/>
       <c r="N78" s="1" t="n"/>
       <c r="O78" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P78" s="1" t="n">
-        <v>-28</v>
+        <v>-42</v>
       </c>
       <c r="Q78" s="1" t="n">
-        <v>-26.975</v>
+        <v>-48.265</v>
       </c>
       <c r="R78" s="1" t="n">
-        <v>1.025</v>
+        <v>-6.265</v>
       </c>
       <c r="S78" s="1" t="n"/>
       <c r="T78" s="1" t="n"/>
@@ -10808,18 +10772,10 @@
       <c r="L79" s="1" t="n"/>
       <c r="M79" s="1" t="n"/>
       <c r="N79" s="1" t="n"/>
-      <c r="O79" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="P79" s="1" t="n">
-        <v>-36</v>
-      </c>
-      <c r="Q79" s="1" t="n">
-        <v>-35.535</v>
-      </c>
-      <c r="R79" s="1" t="n">
-        <v>0.465</v>
-      </c>
+      <c r="O79" s="1" t="n"/>
+      <c r="P79" s="1" t="n"/>
+      <c r="Q79" s="1" t="n"/>
+      <c r="R79" s="1" t="n"/>
       <c r="S79" s="1" t="n"/>
       <c r="T79" s="1" t="n"/>
       <c r="U79" s="1" t="n"/>
@@ -10845,18 +10801,10 @@
       <c r="L80" s="1" t="n"/>
       <c r="M80" s="1" t="n"/>
       <c r="N80" s="1" t="n"/>
-      <c r="O80" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="P80" s="1" t="n">
-        <v>-44</v>
-      </c>
-      <c r="Q80" s="1" t="n">
-        <v>-44.095</v>
-      </c>
-      <c r="R80" s="1" t="n">
-        <v>-0.095</v>
-      </c>
+      <c r="O80" s="1" t="n"/>
+      <c r="P80" s="1" t="n"/>
+      <c r="Q80" s="1" t="n"/>
+      <c r="R80" s="1" t="n"/>
       <c r="S80" s="1" t="n"/>
       <c r="T80" s="1" t="n"/>
       <c r="U80" s="1" t="n"/>
@@ -10926,56 +10874,24 @@
       <c r="AA82" s="1" t="n"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D83" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="H83" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="A83" s="1" t="n"/>
+      <c r="B83" s="1" t="n"/>
+      <c r="C83" s="1" t="n"/>
+      <c r="D83" s="1" t="n"/>
+      <c r="E83" s="1" t="n"/>
+      <c r="F83" s="1" t="n"/>
+      <c r="G83" s="1" t="n"/>
+      <c r="H83" s="1" t="n"/>
       <c r="I83" s="1" t="n"/>
-      <c r="J83" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M83" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J83" s="1" t="n"/>
+      <c r="K83" s="1" t="n"/>
+      <c r="L83" s="1" t="n"/>
+      <c r="M83" s="1" t="n"/>
       <c r="N83" s="1" t="n"/>
-      <c r="O83" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P83" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="Q83" s="1" t="n">
-        <v>35.735</v>
-      </c>
-      <c r="R83" s="1" t="n">
-        <v>-6.265</v>
-      </c>
+      <c r="O83" s="1" t="n"/>
+      <c r="P83" s="1" t="n"/>
+      <c r="Q83" s="1" t="n"/>
+      <c r="R83" s="1" t="n"/>
       <c r="S83" s="1" t="n"/>
       <c r="T83" s="1" t="n"/>
       <c r="U83" s="1" t="n"/>
@@ -10996,31 +10912,15 @@
       <c r="G84" s="1" t="n"/>
       <c r="H84" s="1" t="n"/>
       <c r="I84" s="1" t="n"/>
-      <c r="J84" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K84" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L84" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M84" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J84" s="1" t="n"/>
+      <c r="K84" s="1" t="n"/>
+      <c r="L84" s="1" t="n"/>
+      <c r="M84" s="1" t="n"/>
       <c r="N84" s="1" t="n"/>
-      <c r="O84" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P84" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q84" s="1" t="n">
-        <v>35.335</v>
-      </c>
-      <c r="R84" s="1" t="n">
-        <v>5.335</v>
-      </c>
+      <c r="O84" s="1" t="n"/>
+      <c r="P84" s="1" t="n"/>
+      <c r="Q84" s="1" t="n"/>
+      <c r="R84" s="1" t="n"/>
       <c r="S84" s="1" t="n"/>
       <c r="T84" s="1" t="n"/>
       <c r="U84" s="1" t="n"/>
@@ -11041,31 +10941,15 @@
       <c r="G85" s="1" t="n"/>
       <c r="H85" s="1" t="n"/>
       <c r="I85" s="1" t="n"/>
-      <c r="J85" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K85" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M85" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J85" s="1" t="n"/>
+      <c r="K85" s="1" t="n"/>
+      <c r="L85" s="1" t="n"/>
+      <c r="M85" s="1" t="n"/>
       <c r="N85" s="1" t="n"/>
-      <c r="O85" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P85" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="Q85" s="1" t="n">
-        <v>12.045</v>
-      </c>
-      <c r="R85" s="1" t="n">
-        <v>-5.955</v>
-      </c>
+      <c r="O85" s="1" t="n"/>
+      <c r="P85" s="1" t="n"/>
+      <c r="Q85" s="1" t="n"/>
+      <c r="R85" s="1" t="n"/>
       <c r="S85" s="1" t="n"/>
       <c r="T85" s="1" t="n"/>
       <c r="U85" s="1" t="n"/>
@@ -11086,31 +10970,15 @@
       <c r="G86" s="1" t="n"/>
       <c r="H86" s="1" t="n"/>
       <c r="I86" s="1" t="n"/>
-      <c r="J86" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K86" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L86" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M86" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="J86" s="1" t="n"/>
+      <c r="K86" s="1" t="n"/>
+      <c r="L86" s="1" t="n"/>
+      <c r="M86" s="1" t="n"/>
       <c r="N86" s="1" t="n"/>
-      <c r="O86" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P86" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q86" s="1" t="n">
-        <v>11.645</v>
-      </c>
-      <c r="R86" s="1" t="n">
-        <v>5.645</v>
-      </c>
+      <c r="O86" s="1" t="n"/>
+      <c r="P86" s="1" t="n"/>
+      <c r="Q86" s="1" t="n"/>
+      <c r="R86" s="1" t="n"/>
       <c r="S86" s="1" t="n"/>
       <c r="T86" s="1" t="n"/>
       <c r="U86" s="1" t="n"/>
@@ -11136,18 +11004,10 @@
       <c r="L87" s="1" t="n"/>
       <c r="M87" s="1" t="n"/>
       <c r="N87" s="1" t="n"/>
-      <c r="O87" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P87" s="1" t="n">
-        <v>-6</v>
-      </c>
-      <c r="Q87" s="1" t="n">
-        <v>-11.645</v>
-      </c>
-      <c r="R87" s="1" t="n">
-        <v>-5.645</v>
-      </c>
+      <c r="O87" s="1" t="n"/>
+      <c r="P87" s="1" t="n"/>
+      <c r="Q87" s="1" t="n"/>
+      <c r="R87" s="1" t="n"/>
       <c r="S87" s="1" t="n"/>
       <c r="T87" s="1" t="n"/>
       <c r="U87" s="1" t="n"/>
@@ -11173,18 +11033,10 @@
       <c r="L88" s="1" t="n"/>
       <c r="M88" s="1" t="n"/>
       <c r="N88" s="1" t="n"/>
-      <c r="O88" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="P88" s="1" t="n">
-        <v>-18</v>
-      </c>
-      <c r="Q88" s="1" t="n">
-        <v>-12.045</v>
-      </c>
-      <c r="R88" s="1" t="n">
-        <v>5.955</v>
-      </c>
+      <c r="O88" s="1" t="n"/>
+      <c r="P88" s="1" t="n"/>
+      <c r="Q88" s="1" t="n"/>
+      <c r="R88" s="1" t="n"/>
       <c r="S88" s="1" t="n"/>
       <c r="T88" s="1" t="n"/>
       <c r="U88" s="1" t="n"/>
@@ -11210,18 +11062,10 @@
       <c r="L89" s="1" t="n"/>
       <c r="M89" s="1" t="n"/>
       <c r="N89" s="1" t="n"/>
-      <c r="O89" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="P89" s="1" t="n">
-        <v>-30</v>
-      </c>
-      <c r="Q89" s="1" t="n">
-        <v>-35.335</v>
-      </c>
-      <c r="R89" s="1" t="n">
-        <v>-5.335</v>
-      </c>
+      <c r="O89" s="1" t="n"/>
+      <c r="P89" s="1" t="n"/>
+      <c r="Q89" s="1" t="n"/>
+      <c r="R89" s="1" t="n"/>
       <c r="S89" s="1" t="n"/>
       <c r="T89" s="1" t="n"/>
       <c r="U89" s="1" t="n"/>
@@ -11247,18 +11091,10 @@
       <c r="L90" s="1" t="n"/>
       <c r="M90" s="1" t="n"/>
       <c r="N90" s="1" t="n"/>
-      <c r="O90" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="P90" s="1" t="n">
-        <v>-42</v>
-      </c>
-      <c r="Q90" s="1" t="n">
-        <v>-35.735</v>
-      </c>
-      <c r="R90" s="1" t="n">
-        <v>6.265</v>
-      </c>
+      <c r="O90" s="1" t="n"/>
+      <c r="P90" s="1" t="n"/>
+      <c r="Q90" s="1" t="n"/>
+      <c r="R90" s="1" t="n"/>
       <c r="S90" s="1" t="n"/>
       <c r="T90" s="1" t="n"/>
       <c r="U90" s="1" t="n"/>

</xml_diff>